<commit_message>
Server Refactoring 후 오류 수정
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Character_Stat.xlsx
+++ b/Server/Server/GameData/Character_Stat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\프로젝트\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FestivalTownProject\Server\Server\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579263B2-3E4F-4F7E-93E2-A579EFDDDE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF888004-7C1E-496A-A9BF-9E2392DBBF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{2AE69B0B-1D43-4C54-8DE1-FC8FE06F0720}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2AE69B0B-1D43-4C54-8DE1-FC8FE06F0720}"/>
   </bookViews>
   <sheets>
     <sheet name="Character_Attack_Variable" sheetId="8" r:id="rId1"/>
@@ -324,7 +324,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -340,44 +340,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -394,10 +382,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -723,21 +707,21 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="11"/>
       <c r="C1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -745,7 +729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -753,7 +737,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -761,7 +745,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -769,7 +753,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -777,16 +761,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.45">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="11"/>
       <c r="C7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -794,7 +778,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -802,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -810,7 +794,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -835,100 +819,91 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="E29" sqref="E29"/>
-      <selection pane="topRight" activeCell="I14" sqref="I14"/>
+      <selection pane="topRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.08203125" customWidth="1"/>
-    <col min="2" max="2" width="13.08203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.9140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.125" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.4140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.58203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.625" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.4140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.58203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.58203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:39" s="5" customFormat="1" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="8" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="8" t="s">
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="15"/>
-    </row>
-    <row r="2" spans="1:39" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AM1" s="8"/>
+    </row>
+    <row r="2" spans="1:39" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1019,17 +994,17 @@
       <c r="AD2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="16"/>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.45">
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
+      <c r="AM2" s="9"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -1075,58 +1050,26 @@
         <f>F3*Character_Attack_Variable!B10</f>
         <v>15</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3">
         <f>F3*Character_Attack_Variable!B11</f>
         <v>20</v>
       </c>
       <c r="W3">
         <v>5</v>
       </c>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="14"/>
-      <c r="AM3" s="17"/>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="14"/>
-      <c r="AJ4" s="14"/>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
-      <c r="AM4" s="17"/>
-    </row>
-    <row r="9" spans="1:39" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="T9" s="12"/>
-    </row>
-    <row r="10" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="T10" s="3"/>
-    </row>
-    <row r="11" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="T11" s="3"/>
-    </row>
-    <row r="12" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="I12" s="11"/>
-      <c r="K12" s="3"/>
-      <c r="T12" s="3"/>
+      <c r="AM3" s="10"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AM4" s="10"/>
+    </row>
+    <row r="9" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="I12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>